<commit_message>
Adding in implementations of other scraping functions
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>name</t>
   </si>
@@ -25,13 +25,151 @@
     <t>record</t>
   </si>
   <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>hometown</t>
+  </si>
+  <si>
+    <t>trains_at</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>octagon_debut</t>
+  </si>
+  <si>
+    <t>reach</t>
+  </si>
+  <si>
+    <t>leg_reach</t>
+  </si>
+  <si>
+    <t>significant_strikes_landed</t>
+  </si>
+  <si>
+    <t>significant_strikes_attempted</t>
+  </si>
+  <si>
+    <t>signicant_strike_accuracy</t>
+  </si>
+  <si>
+    <t>takedowns_landed</t>
+  </si>
+  <si>
+    <t>takedowns_attempted</t>
+  </si>
+  <si>
+    <t>takedowns_accuracy</t>
+  </si>
+  <si>
     <t>Khabib Nurmagomedov</t>
   </si>
   <si>
+    <t>Jon Jones</t>
+  </si>
+  <si>
     <t>The Eagle</t>
   </si>
   <si>
+    <t>Bones</t>
+  </si>
+  <si>
     <t>29-0-0 (W-L-D)</t>
+  </si>
+  <si>
+    <t>26-1-0 (W-L-D)</t>
+  </si>
+  <si>
+    <t>Retired</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Dagestan Republic, Russia</t>
+  </si>
+  <si>
+    <t>Rochester, United States</t>
+  </si>
+  <si>
+    <t>AKA (American Kickboxing Academy) San Jose</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>70.00</t>
+  </si>
+  <si>
+    <t>76.00</t>
+  </si>
+  <si>
+    <t>155.00</t>
+  </si>
+  <si>
+    <t>205.00</t>
+  </si>
+  <si>
+    <t>Jan. 21, 2012</t>
+  </si>
+  <si>
+    <t>Aug. 09, 2008</t>
+  </si>
+  <si>
+    <t>84.50</t>
+  </si>
+  <si>
+    <t>40.00</t>
+  </si>
+  <si>
+    <t>45.00</t>
+  </si>
+  <si>
+    <t>705</t>
+  </si>
+  <si>
+    <t>1463</t>
+  </si>
+  <si>
+    <t>1444</t>
+  </si>
+  <si>
+    <t>2526</t>
+  </si>
+  <si>
+    <t>49%</t>
+  </si>
+  <si>
+    <t>58%</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>48%</t>
+  </si>
+  <si>
+    <t>44%</t>
   </si>
 </sst>
 </file>
@@ -389,13 +527,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:19">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,19 +543,165 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>47</v>
+      </c>
+      <c r="R3" t="s">
+        <v>49</v>
+      </c>
+      <c r="S3" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>